<commit_message>
=Added count of length of glosses
Former-commit-id: 0f66c4dcda32d7f7d62bfe723066ccdc09c9a5a7 [formerly 3e6ccd87737141b87cecd53a4103ab2f601cf7fe]
Former-commit-id: b6ba27488cb9c103b975547cbaa0d23e9f797cd9
Former-commit-id: 46082a21c2013553943ffe8fb999b1d878224801
</commit_message>
<xml_diff>
--- a/Results/Chapter15_ReRun_withTime&TestSet/Experiments_Chapter15_all.xlsx
+++ b/Results/Chapter15_ReRun_withTime&TestSet/Experiments_Chapter15_all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea\Documents\1_TheWorkingDesk\ALMA_PhD\Code\MultiSense_LanguageModel\Results\Chapter15_ReRun_withTime&amp;TestSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C9D893-B6E5-4514-AF11-DCA1102B4734}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C82BE5-78DD-4252-A242-F5AD57810B6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11196" yWindow="12" windowWidth="11772" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11544" yWindow="96" windowWidth="11460" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="53">
   <si>
     <t>Vanilla GRU</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Self Attention</t>
   </si>
   <si>
-    <t>On the validation set:</t>
-  </si>
-  <si>
     <t>SelectK</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>108779.83</t>
   </si>
   <si>
-    <t>(taken from the old runs because I used 2 GPUs for this one)</t>
-  </si>
-  <si>
     <t>25155.54</t>
   </si>
   <si>
@@ -176,13 +170,37 @@
   </si>
   <si>
     <t>37810.48</t>
+  </si>
+  <si>
+    <t>70306.61</t>
+  </si>
+  <si>
+    <t>MFS</t>
+  </si>
+  <si>
+    <t>28173.46</t>
+  </si>
+  <si>
+    <t>57434.16</t>
+  </si>
+  <si>
+    <t>57434.45</t>
+  </si>
+  <si>
+    <t>27390.02</t>
+  </si>
+  <si>
+    <t>18194.21</t>
+  </si>
+  <si>
+    <t>51686.13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,14 +210,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -227,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -235,7 +245,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,30 +525,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:X56"/>
+  <dimension ref="B1:U60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
       <c r="I5" s="4" t="s">
         <v>10</v>
       </c>
@@ -548,16 +557,14 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="P5" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
       <c r="I6" s="4" t="s">
         <v>14</v>
       </c>
@@ -568,18 +575,14 @@
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
-      <c r="P6" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
-      <c r="S6" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>1</v>
       </c>
@@ -590,7 +593,7 @@
         <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
@@ -611,151 +614,156 @@
         <v>13</v>
       </c>
       <c r="P7" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>12</v>
-      </c>
-      <c r="R7" t="s">
-        <v>13</v>
-      </c>
-      <c r="S7" t="s">
-        <v>11</v>
-      </c>
-      <c r="T7" t="s">
-        <v>12</v>
-      </c>
-      <c r="U7" t="s">
-        <v>13</v>
-      </c>
-      <c r="W7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="X8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9">
-        <v>4971</v>
-      </c>
-      <c r="J9">
-        <v>88480</v>
-      </c>
-      <c r="K9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2">
+        <v>9192</v>
+      </c>
+      <c r="J9" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K9" s="2">
         <f>ROUND(I9/J9,3)</f>
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>25353</v>
-      </c>
-      <c r="N9">
+        <v>0.104</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N9" s="2">
         <f>ROUND(L9/M9,3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10">
+      <c r="O9" s="2"/>
+      <c r="P9" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2">
         <v>9192</v>
       </c>
-      <c r="J10">
-        <v>88480</v>
-      </c>
-      <c r="K10">
+      <c r="J10" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K10" s="2">
         <f>ROUND(I10/J10,3)</f>
         <v>0.104</v>
       </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>25353</v>
-      </c>
-      <c r="N10">
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N10" s="2">
         <f>ROUND(L10/M10,3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12">
+      <c r="O10" s="2"/>
+      <c r="P10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2">
         <v>1</v>
       </c>
-      <c r="I12">
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2">
         <v>19036</v>
       </c>
-      <c r="J12">
-        <v>88480</v>
-      </c>
-      <c r="K12">
+      <c r="J12" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K12" s="2">
         <f>ROUND(I12/J12,3)</f>
         <v>0.215</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="2">
         <v>315</v>
       </c>
-      <c r="M12">
-        <v>25353</v>
-      </c>
-      <c r="N12">
+      <c r="M12" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N12" s="2">
         <f>ROUND(L12/M12,3)</f>
         <v>1.2E-2</v>
       </c>
-      <c r="W12" t="s">
+      <c r="P12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2">
+        <v>10699</v>
+      </c>
+      <c r="J13" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" ref="K13:K22" si="0">ROUND(I13/J13,3)</f>
+        <v>0.121</v>
+      </c>
+      <c r="L13" s="2">
+        <v>172</v>
+      </c>
+      <c r="M13" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" ref="N13:N22" si="1">ROUND(L13/M13,3)</f>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="P13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <v>5</v>
-      </c>
-      <c r="I13">
-        <v>10699</v>
-      </c>
-      <c r="J13">
-        <v>88480</v>
-      </c>
-      <c r="K13">
-        <f t="shared" ref="K13:K56" si="0">ROUND(I13/J13,3)</f>
-        <v>0.121</v>
-      </c>
-      <c r="L13">
-        <v>172</v>
-      </c>
-      <c r="M13">
-        <v>25353</v>
-      </c>
-      <c r="N13">
-        <f t="shared" ref="N13:N56" si="1">ROUND(L13/M13,3)</f>
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="W13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>2</v>
       </c>
@@ -782,11 +790,11 @@
         <f t="shared" si="1"/>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="W14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="P14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>2</v>
       </c>
@@ -813,73 +821,79 @@
         <f t="shared" si="1"/>
         <v>1E-3</v>
       </c>
-      <c r="W15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="D16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16">
+      <c r="P15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2">
         <v>1</v>
       </c>
-      <c r="I16">
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2">
         <v>19178</v>
       </c>
-      <c r="J16">
-        <v>88480</v>
-      </c>
-      <c r="K16">
+      <c r="J16" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K16" s="2">
         <f t="shared" si="0"/>
         <v>0.217</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="2">
         <v>340</v>
       </c>
-      <c r="M16">
-        <v>25353</v>
-      </c>
-      <c r="N16">
+      <c r="M16" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N16" s="2">
         <f t="shared" si="1"/>
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="W16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17">
+      <c r="P16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2">
         <v>5</v>
       </c>
-      <c r="I17">
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2">
         <v>11311</v>
       </c>
-      <c r="J17">
-        <v>88480</v>
-      </c>
-      <c r="K17">
+      <c r="J17" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K17" s="2">
         <f t="shared" si="0"/>
         <v>0.128</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="2">
         <v>145</v>
       </c>
-      <c r="M17">
-        <v>25353</v>
-      </c>
-      <c r="N17">
+      <c r="M17" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N17" s="2">
         <f t="shared" si="1"/>
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="W17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="P17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>3</v>
       </c>
@@ -906,11 +920,11 @@
         <f t="shared" si="1"/>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="W18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="P18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>3</v>
       </c>
@@ -937,164 +951,81 @@
         <f t="shared" si="1"/>
         <v>2E-3</v>
       </c>
-      <c r="W19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+      <c r="P19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2">
+        <v>18528</v>
+      </c>
+      <c r="J21" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="L21" s="2">
+        <v>268</v>
+      </c>
+      <c r="M21" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="P21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2">
+        <v>18637</v>
+      </c>
+      <c r="J22" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="L22" s="2">
+        <v>293</v>
+      </c>
+      <c r="M22" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N22" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D21" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>10</v>
-      </c>
-      <c r="H21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21">
-        <v>17300</v>
-      </c>
-      <c r="J21">
-        <v>88480</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="0"/>
-        <v>0.19600000000000001</v>
-      </c>
-      <c r="L21">
-        <v>62</v>
-      </c>
-      <c r="M21">
-        <v>25353</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="1"/>
-        <v>2E-3</v>
-      </c>
-      <c r="W21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D22" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>20</v>
-      </c>
-      <c r="H22" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22">
-        <v>18006</v>
-      </c>
-      <c r="J22">
-        <v>88480</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="0"/>
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="L22">
-        <v>225</v>
-      </c>
-      <c r="M22">
-        <v>25353</v>
-      </c>
-      <c r="N22">
-        <f t="shared" si="1"/>
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="W22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23">
-        <v>5</v>
-      </c>
-      <c r="G23">
-        <v>10</v>
-      </c>
-      <c r="H23" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23">
-        <v>11039</v>
-      </c>
-      <c r="J23">
-        <v>88480</v>
-      </c>
-      <c r="K23">
-        <f>ROUND(I23/J23,3)</f>
-        <v>0.125</v>
-      </c>
-      <c r="L23">
-        <v>34</v>
-      </c>
-      <c r="M23">
-        <v>25353</v>
-      </c>
-      <c r="N23">
-        <f>ROUND(L23/M23,3)</f>
-        <v>1E-3</v>
-      </c>
-      <c r="W23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D24" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24">
-        <v>5</v>
-      </c>
-      <c r="G24">
-        <v>20</v>
-      </c>
-      <c r="H24" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24">
-        <v>12366</v>
-      </c>
-      <c r="J24">
-        <v>88480</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="0"/>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="L24">
-        <v>41</v>
-      </c>
-      <c r="M24">
-        <v>25353</v>
-      </c>
-      <c r="N24">
-        <f t="shared" si="1"/>
-        <v>2E-3</v>
-      </c>
-      <c r="W24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1106,69 +1037,70 @@
         <v>16</v>
       </c>
       <c r="I25">
-        <v>17234</v>
+        <v>17300</v>
       </c>
       <c r="J25">
         <v>88480</v>
       </c>
       <c r="K25">
-        <f>ROUND(I25/J25,3)</f>
-        <v>0.19500000000000001</v>
+        <f t="shared" ref="K25:K32" si="2">ROUND(I25/J25,3)</f>
+        <v>0.19600000000000001</v>
       </c>
       <c r="L25">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="M25">
         <v>25353</v>
       </c>
       <c r="N25">
-        <f>ROUND(L25/M25,3)</f>
+        <f t="shared" ref="N25:N32" si="3">ROUND(L25/M25,3)</f>
         <v>2E-3</v>
       </c>
-      <c r="W25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D26" t="s">
-        <v>3</v>
-      </c>
-      <c r="F26">
+      <c r="P25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2">
         <v>1</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="2">
         <v>20</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I26">
-        <v>18106</v>
-      </c>
-      <c r="J26">
-        <v>88480</v>
-      </c>
-      <c r="K26">
-        <f>ROUND(I26/J26,3)</f>
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="L26">
-        <v>282</v>
-      </c>
-      <c r="M26">
-        <v>25353</v>
-      </c>
-      <c r="N26">
-        <f>ROUND(L26/M26,3)</f>
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="W26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="I26" s="2">
+        <v>18006</v>
+      </c>
+      <c r="J26" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="2"/>
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="L26" s="2">
+        <v>225</v>
+      </c>
+      <c r="M26" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" si="3"/>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="P26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27">
         <v>5</v>
@@ -1180,289 +1112,330 @@
         <v>16</v>
       </c>
       <c r="I27">
+        <v>11039</v>
+      </c>
+      <c r="J27">
+        <v>88480</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="L27">
+        <v>34</v>
+      </c>
+      <c r="M27">
+        <v>25353</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="3"/>
+        <v>1E-3</v>
+      </c>
+      <c r="P27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2">
+        <v>5</v>
+      </c>
+      <c r="G28" s="2">
+        <v>20</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="2">
+        <v>12366</v>
+      </c>
+      <c r="J28" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K28" s="2">
+        <f t="shared" si="2"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L28" s="2">
+        <v>41</v>
+      </c>
+      <c r="M28" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" si="3"/>
+        <v>2E-3</v>
+      </c>
+      <c r="P28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>10</v>
+      </c>
+      <c r="H29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29">
+        <v>17234</v>
+      </c>
+      <c r="J29">
+        <v>88480</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="2"/>
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="L29">
+        <v>47</v>
+      </c>
+      <c r="M29">
+        <v>25353</v>
+      </c>
+      <c r="N29">
+        <f>ROUND(L29/M29,3)</f>
+        <v>2E-3</v>
+      </c>
+      <c r="P29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2">
+        <v>20</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="2">
+        <v>18106</v>
+      </c>
+      <c r="J30" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K30" s="2">
+        <f t="shared" si="2"/>
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="L30" s="2">
+        <v>282</v>
+      </c>
+      <c r="M30" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="P30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+      <c r="G31">
+        <v>10</v>
+      </c>
+      <c r="H31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31">
         <v>5967</v>
       </c>
-      <c r="J27">
-        <v>88480</v>
-      </c>
-      <c r="K27">
-        <f>ROUND(I27/J27,3)</f>
+      <c r="J31">
+        <v>88480</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="2"/>
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="L27">
+      <c r="L31">
         <v>52</v>
       </c>
-      <c r="M27">
-        <v>25353</v>
-      </c>
-      <c r="N27">
-        <f>ROUND(L27/M27,3)</f>
+      <c r="M31">
+        <v>25353</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="3"/>
         <v>2E-3</v>
       </c>
-      <c r="W27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D28" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28">
+      <c r="P31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2">
         <v>5</v>
       </c>
-      <c r="G28">
+      <c r="G32" s="2">
         <v>20</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I28">
+      <c r="I32" s="2">
         <v>7653</v>
       </c>
-      <c r="J28">
-        <v>88480</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="0"/>
+      <c r="J32" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" si="2"/>
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="L28">
+      <c r="L32" s="2">
         <v>161</v>
       </c>
-      <c r="M28">
-        <v>25353</v>
-      </c>
-      <c r="N28">
-        <f t="shared" si="1"/>
+      <c r="M32" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="3"/>
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="W28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
+      <c r="P32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
         <v>7</v>
       </c>
-      <c r="D30" t="s">
-        <v>2</v>
-      </c>
-      <c r="F30">
+      <c r="D34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2">
         <v>1</v>
       </c>
-      <c r="G30">
+      <c r="G34" s="2">
         <v>10</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H34" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I30">
+      <c r="I34" s="2">
         <v>13009</v>
       </c>
-      <c r="J30">
-        <v>88480</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="0"/>
+      <c r="J34" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K34" s="2">
+        <f t="shared" ref="K34:K41" si="4">ROUND(I34/J34,3)</f>
         <v>0.14699999999999999</v>
       </c>
-      <c r="L30">
+      <c r="L34" s="2">
         <v>14</v>
       </c>
-      <c r="M30">
-        <v>25353</v>
-      </c>
-      <c r="N30">
-        <f t="shared" si="1"/>
+      <c r="M34" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N34" s="2">
+        <f t="shared" ref="N34:N41" si="5">ROUND(L34/M34,3)</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D31" t="s">
-        <v>2</v>
-      </c>
-      <c r="F31">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35">
         <v>1</v>
       </c>
-      <c r="G31">
+      <c r="G35">
         <v>20</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H35" t="s">
         <v>17</v>
       </c>
-      <c r="I31">
+      <c r="I35">
         <v>12625</v>
       </c>
-      <c r="J31">
-        <v>88480</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="0"/>
+      <c r="J35">
+        <v>88480</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="4"/>
         <v>0.14299999999999999</v>
       </c>
-      <c r="L31">
+      <c r="L35">
         <v>16</v>
       </c>
-      <c r="M31">
-        <v>25353</v>
-      </c>
-      <c r="N31">
-        <f t="shared" si="1"/>
+      <c r="M35">
+        <v>25353</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="5"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D32" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1">
         <v>5</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G36" s="1">
         <v>10</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="H36" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5">
-        <v>88480</v>
-      </c>
-      <c r="K32" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5">
-        <v>25353</v>
-      </c>
-      <c r="N32" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D33" t="s">
-        <v>2</v>
-      </c>
-      <c r="F33">
-        <v>5</v>
-      </c>
-      <c r="G33">
-        <v>20</v>
-      </c>
-      <c r="H33" t="s">
-        <v>17</v>
-      </c>
-      <c r="J33">
-        <v>88480</v>
-      </c>
-      <c r="K33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M33">
-        <v>25353</v>
-      </c>
-      <c r="N33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D34" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5">
-        <v>1</v>
-      </c>
-      <c r="G34" s="5">
-        <v>10</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5">
-        <v>88480</v>
-      </c>
-      <c r="K34" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5">
-        <v>25353</v>
-      </c>
-      <c r="N34" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D35" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5">
-        <v>1</v>
-      </c>
-      <c r="G35" s="5">
-        <v>20</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5">
-        <v>88480</v>
-      </c>
-      <c r="K35" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5">
-        <v>25353</v>
-      </c>
-      <c r="N35" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F36">
-        <v>5</v>
-      </c>
-      <c r="G36">
-        <v>10</v>
-      </c>
-      <c r="H36" t="s">
-        <v>17</v>
-      </c>
-      <c r="J36">
-        <v>88480</v>
-      </c>
-      <c r="K36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M36">
-        <v>25353</v>
-      </c>
-      <c r="N36">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="I36" s="1">
+        <v>4058</v>
+      </c>
+      <c r="J36" s="1">
+        <v>88480</v>
+      </c>
+      <c r="K36" s="1">
+        <f t="shared" si="4"/>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="L36" s="1">
+        <v>15</v>
+      </c>
+      <c r="M36" s="1">
+        <v>25353</v>
+      </c>
+      <c r="N36" s="1">
+        <f t="shared" si="5"/>
+        <v>1E-3</v>
+      </c>
+      <c r="P36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37">
         <v>5</v>
@@ -1477,277 +1450,265 @@
         <v>88480</v>
       </c>
       <c r="K37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M37">
         <v>25353</v>
       </c>
       <c r="N37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>18</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2">
+        <v>1</v>
+      </c>
+      <c r="G38" s="2">
+        <v>10</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I38" s="2">
+        <v>11940</v>
+      </c>
+      <c r="J38" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="4"/>
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="L38" s="2">
+        <v>12</v>
+      </c>
+      <c r="M38" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1">
+        <v>20</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="1">
+        <v>12061</v>
+      </c>
+      <c r="J39" s="1">
+        <v>88480</v>
+      </c>
+      <c r="K39" s="1">
+        <f t="shared" si="4"/>
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="L39" s="1">
+        <v>15</v>
+      </c>
+      <c r="M39" s="1">
+        <v>25353</v>
+      </c>
+      <c r="N39" s="1">
+        <f t="shared" si="5"/>
+        <v>1E-3</v>
+      </c>
+      <c r="P39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G40">
         <v>10</v>
       </c>
       <c r="H40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40">
-        <v>16821</v>
+        <v>17</v>
       </c>
       <c r="J40">
         <v>88480</v>
       </c>
       <c r="K40">
-        <f t="shared" si="0"/>
-        <v>0.19</v>
-      </c>
-      <c r="L40">
-        <v>171</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="M40">
         <v>25353</v>
       </c>
       <c r="N40">
-        <f t="shared" si="1"/>
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="W40" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G41">
         <v>20</v>
       </c>
       <c r="H41" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41">
+        <v>88480</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>25353</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
+      <c r="G44" s="2">
+        <v>10</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I41">
+      <c r="I44" s="2">
+        <v>16821</v>
+      </c>
+      <c r="J44" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K44" s="2">
+        <f t="shared" ref="K44:K51" si="6">ROUND(I44/J44,3)</f>
+        <v>0.19</v>
+      </c>
+      <c r="L44" s="2">
+        <v>171</v>
+      </c>
+      <c r="M44" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N44" s="2">
+        <f t="shared" ref="N44:N51" si="7">ROUND(L44/M44,3)</f>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="P44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>20</v>
+      </c>
+      <c r="H45" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45">
         <v>16417</v>
       </c>
-      <c r="J41">
-        <v>88480</v>
-      </c>
-      <c r="K41">
-        <f t="shared" si="0"/>
+      <c r="J45">
+        <v>88480</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="6"/>
         <v>0.186</v>
       </c>
-      <c r="L41">
+      <c r="L45">
         <v>163</v>
       </c>
-      <c r="M41">
-        <v>25353</v>
-      </c>
-      <c r="N41">
-        <f t="shared" si="1"/>
+      <c r="M45">
+        <v>25353</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="7"/>
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D42" t="s">
-        <v>2</v>
-      </c>
-      <c r="F42">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2">
         <v>5</v>
       </c>
-      <c r="G42">
+      <c r="G46" s="2">
         <v>10</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H46" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I42">
+      <c r="I46" s="2">
         <v>7300</v>
       </c>
-      <c r="J42">
-        <v>88480</v>
-      </c>
-      <c r="K42">
-        <f t="shared" si="0"/>
+      <c r="J46" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K46" s="2">
+        <f t="shared" si="6"/>
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L42">
+      <c r="L46" s="2">
         <v>106</v>
       </c>
-      <c r="M42">
-        <v>25353</v>
-      </c>
-      <c r="N42">
-        <f t="shared" si="1"/>
+      <c r="M46" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N46" s="2">
+        <f t="shared" si="7"/>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="W42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D43" t="s">
-        <v>2</v>
-      </c>
-      <c r="F43">
-        <v>5</v>
-      </c>
-      <c r="G43">
-        <v>20</v>
-      </c>
-      <c r="H43" t="s">
-        <v>16</v>
-      </c>
-      <c r="I43">
-        <v>7042</v>
-      </c>
-      <c r="J43">
-        <v>88480</v>
-      </c>
-      <c r="K43">
-        <f t="shared" si="0"/>
-        <v>0.08</v>
-      </c>
-      <c r="L43">
-        <v>29</v>
-      </c>
-      <c r="M43">
-        <v>25353</v>
-      </c>
-      <c r="N43">
-        <f t="shared" si="1"/>
-        <v>1E-3</v>
-      </c>
-      <c r="W43" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D44" t="s">
-        <v>3</v>
-      </c>
-      <c r="F44">
-        <v>1</v>
-      </c>
-      <c r="G44">
-        <v>10</v>
-      </c>
-      <c r="H44" t="s">
-        <v>16</v>
-      </c>
-      <c r="I44">
-        <v>16989</v>
-      </c>
-      <c r="J44">
-        <v>88480</v>
-      </c>
-      <c r="K44">
-        <f t="shared" si="0"/>
-        <v>0.192</v>
-      </c>
-      <c r="L44">
-        <v>237</v>
-      </c>
-      <c r="M44">
-        <v>25353</v>
-      </c>
-      <c r="N44">
-        <f t="shared" si="1"/>
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="W44" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D45" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5">
-        <v>1</v>
-      </c>
-      <c r="G45" s="5">
-        <v>20</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I45" s="5">
-        <v>0</v>
-      </c>
-      <c r="J45" s="5">
-        <v>88480</v>
-      </c>
-      <c r="K45" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L45" s="5">
-        <v>0</v>
-      </c>
-      <c r="M45" s="5">
-        <v>25353</v>
-      </c>
-      <c r="N45" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="D46" t="s">
-        <v>3</v>
-      </c>
-      <c r="F46">
-        <v>5</v>
-      </c>
-      <c r="G46">
-        <v>10</v>
-      </c>
-      <c r="H46" t="s">
-        <v>16</v>
-      </c>
-      <c r="I46">
-        <v>7769</v>
-      </c>
-      <c r="J46">
-        <v>88480</v>
-      </c>
-      <c r="K46">
-        <f t="shared" si="0"/>
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="L46">
-        <v>86</v>
-      </c>
-      <c r="M46">
-        <v>25353</v>
-      </c>
-      <c r="N46">
-        <f t="shared" si="1"/>
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="W46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="P46" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47">
         <v>5</v>
@@ -1759,120 +1720,183 @@
         <v>16</v>
       </c>
       <c r="I47">
+        <v>7042</v>
+      </c>
+      <c r="J47">
+        <v>88480</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="6"/>
+        <v>0.08</v>
+      </c>
+      <c r="L47">
+        <v>29</v>
+      </c>
+      <c r="M47">
+        <v>25353</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="7"/>
+        <v>1E-3</v>
+      </c>
+      <c r="P47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D48" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2">
+        <v>1</v>
+      </c>
+      <c r="G48" s="2">
+        <v>10</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I48" s="2">
+        <v>16989</v>
+      </c>
+      <c r="J48" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K48" s="2">
+        <f t="shared" si="6"/>
+        <v>0.192</v>
+      </c>
+      <c r="L48" s="2">
+        <v>237</v>
+      </c>
+      <c r="M48" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N48" s="2">
+        <f t="shared" si="7"/>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="P48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1">
+        <v>1</v>
+      </c>
+      <c r="G49" s="1">
+        <v>20</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I49" s="1">
+        <v>16563</v>
+      </c>
+      <c r="J49" s="1">
+        <v>88480</v>
+      </c>
+      <c r="K49" s="1">
+        <f t="shared" si="6"/>
+        <v>0.187</v>
+      </c>
+      <c r="L49" s="1">
+        <v>165</v>
+      </c>
+      <c r="M49" s="1">
+        <v>25353</v>
+      </c>
+      <c r="N49" s="1">
+        <f t="shared" si="7"/>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="P49" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2">
+        <v>5</v>
+      </c>
+      <c r="G50" s="2">
+        <v>10</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I50" s="2">
+        <v>7769</v>
+      </c>
+      <c r="J50" s="2">
+        <v>88480</v>
+      </c>
+      <c r="K50" s="2">
+        <f t="shared" si="6"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="L50" s="2">
+        <v>86</v>
+      </c>
+      <c r="M50" s="2">
+        <v>25353</v>
+      </c>
+      <c r="N50" s="2">
+        <f t="shared" si="7"/>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P50" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>3</v>
+      </c>
+      <c r="F51">
+        <v>5</v>
+      </c>
+      <c r="G51">
+        <v>20</v>
+      </c>
+      <c r="H51" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51">
         <v>7435</v>
       </c>
-      <c r="J47">
-        <v>88480</v>
-      </c>
-      <c r="K47">
-        <f t="shared" si="0"/>
+      <c r="J51">
+        <v>88480</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="6"/>
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="L47">
+      <c r="L51">
         <v>40</v>
       </c>
-      <c r="M47">
-        <v>25353</v>
-      </c>
-      <c r="N47">
-        <f t="shared" si="1"/>
+      <c r="M51">
+        <v>25353</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="7"/>
         <v>2E-3</v>
       </c>
-      <c r="W47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D49" t="s">
-        <v>2</v>
-      </c>
-      <c r="H49" t="s">
-        <v>17</v>
-      </c>
-      <c r="J49">
-        <v>88480</v>
-      </c>
-      <c r="K49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M49">
-        <v>25353</v>
-      </c>
-      <c r="N49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D50" t="s">
-        <v>2</v>
-      </c>
-      <c r="H50" t="s">
-        <v>17</v>
-      </c>
-      <c r="J50">
-        <v>88480</v>
-      </c>
-      <c r="K50">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M50">
-        <v>25353</v>
-      </c>
-      <c r="N50">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D51" t="s">
-        <v>2</v>
-      </c>
-      <c r="H51" t="s">
-        <v>17</v>
-      </c>
-      <c r="J51">
-        <v>88480</v>
-      </c>
-      <c r="K51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M51">
-        <v>25353</v>
-      </c>
-      <c r="N51">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H52" t="s">
-        <v>17</v>
-      </c>
-      <c r="J52">
-        <v>88480</v>
-      </c>
-      <c r="K52">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M52">
-        <v>25353</v>
-      </c>
-      <c r="N52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="P51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H53" t="s">
         <v>17</v>
@@ -1881,20 +1905,20 @@
         <v>88480</v>
       </c>
       <c r="K53">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K53:K60" si="8">ROUND(I53/J53,3)</f>
         <v>0</v>
       </c>
       <c r="M53">
         <v>25353</v>
       </c>
       <c r="N53">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="4:14" x14ac:dyDescent="0.3">
+        <f t="shared" ref="N53:N60" si="9">ROUND(L53/M53,3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H54" t="s">
         <v>17</v>
@@ -1903,20 +1927,20 @@
         <v>88480</v>
       </c>
       <c r="K54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M54">
         <v>25353</v>
       </c>
       <c r="N54">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="4:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H55" t="s">
         <v>17</v>
@@ -1925,20 +1949,20 @@
         <v>88480</v>
       </c>
       <c r="K55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M55">
         <v>25353</v>
       </c>
       <c r="N55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="4:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H56" t="s">
         <v>17</v>
@@ -1947,14 +1971,102 @@
         <v>88480</v>
       </c>
       <c r="K56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M56">
         <v>25353</v>
       </c>
       <c r="N56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D57" t="s">
+        <v>3</v>
+      </c>
+      <c r="H57" t="s">
+        <v>17</v>
+      </c>
+      <c r="J57">
+        <v>88480</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M57">
+        <v>25353</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D58" t="s">
+        <v>3</v>
+      </c>
+      <c r="H58" t="s">
+        <v>17</v>
+      </c>
+      <c r="J58">
+        <v>88480</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <v>25353</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>3</v>
+      </c>
+      <c r="H59" t="s">
+        <v>17</v>
+      </c>
+      <c r="J59">
+        <v>88480</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>25353</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
+        <v>3</v>
+      </c>
+      <c r="H60" t="s">
+        <v>17</v>
+      </c>
+      <c r="J60">
+        <v>88480</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <v>25353</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1984,7 +2096,7 @@
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
@@ -1998,7 +2110,7 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -2021,7 +2133,7 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -2052,7 +2164,7 @@
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
@@ -2275,7 +2387,7 @@
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
         <v>3</v>
@@ -2343,7 +2455,7 @@
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
         <v>2</v>
@@ -2373,7 +2485,7 @@
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
         <v>3</v>
@@ -2474,7 +2586,7 @@
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
         <v>2</v>
@@ -2575,7 +2687,7 @@
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" t="s">
         <v>2</v>
@@ -2606,7 +2718,7 @@
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
=Before adding scripts and refactoring for public version
Former-commit-id: 89122ed6f45f16af43876df91037a333978711ff [formerly fb755aa3405c57b6e9f4a6ab2817f7a9166a901d]
Former-commit-id: 8c2ecd89ac2af0f17d345d768da620d429b20cce
Former-commit-id: 77b8efa18b2fdc3fbf08005fb8f3f75642793cda
</commit_message>
<xml_diff>
--- a/Results/Chapter15_ReRun_withTime&TestSet/Experiments_Chapter15_all.xlsx
+++ b/Results/Chapter15_ReRun_withTime&TestSet/Experiments_Chapter15_all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea\Documents\1_TheWorkingDesk\ALMA_PhD\Code\MultiSense_LanguageModel\Results\Chapter15_ReRun_withTime&amp;TestSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C82BE5-78DD-4252-A242-F5AD57810B6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59C336A-47C8-4DBC-A542-58D4C1A646FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11544" yWindow="96" windowWidth="11460" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11724" yWindow="312" windowWidth="11280" windowHeight="12048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:U60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1550,19 +1550,25 @@
       <c r="H40" t="s">
         <v>17</v>
       </c>
+      <c r="I40">
+        <v>2705</v>
+      </c>
       <c r="J40">
         <v>88480</v>
       </c>
       <c r="K40">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.1E-2</v>
+      </c>
+      <c r="L40">
+        <v>15</v>
       </c>
       <c r="M40">
         <v>25353</v>
       </c>
       <c r="N40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.3">

</xml_diff>